<commit_message>
Datos para Google Data Studio
</commit_message>
<xml_diff>
--- a/datos/out/productos_indispensables.xlsx
+++ b/datos/out/productos_indispensables.xlsx
@@ -1924,7 +1924,7 @@
         <v>44623</v>
       </c>
       <c r="F2">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1944,7 +1944,7 @@
         <v>44623</v>
       </c>
       <c r="F3">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1964,7 +1964,7 @@
         <v>44623</v>
       </c>
       <c r="F4">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2124,7 +2124,7 @@
         <v>44623</v>
       </c>
       <c r="F12">
-        <v>113</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2204,7 +2204,7 @@
         <v>44623</v>
       </c>
       <c r="F16">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2224,7 +2224,7 @@
         <v>44623</v>
       </c>
       <c r="F17">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2264,7 +2264,7 @@
         <v>44623</v>
       </c>
       <c r="F19">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2284,7 +2284,7 @@
         <v>44623</v>
       </c>
       <c r="F20">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2304,7 +2304,7 @@
         <v>44623</v>
       </c>
       <c r="F21">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -2344,7 +2344,7 @@
         <v>44623</v>
       </c>
       <c r="F23">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -2444,7 +2444,7 @@
         <v>44623</v>
       </c>
       <c r="F28">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -2464,7 +2464,7 @@
         <v>44623</v>
       </c>
       <c r="F29">
-        <v>190</v>
+        <v>203</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -2484,7 +2484,7 @@
         <v>44623</v>
       </c>
       <c r="F30">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -2524,7 +2524,7 @@
         <v>44623</v>
       </c>
       <c r="F32">
-        <v>840</v>
+        <v>899</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -2564,7 +2564,7 @@
         <v>44623</v>
       </c>
       <c r="F34">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -2644,7 +2644,7 @@
         <v>44623</v>
       </c>
       <c r="F38">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -2664,7 +2664,7 @@
         <v>44623</v>
       </c>
       <c r="F39">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -2704,7 +2704,7 @@
         <v>44623</v>
       </c>
       <c r="F41">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -2744,7 +2744,7 @@
         <v>44623</v>
       </c>
       <c r="F43">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -2764,7 +2764,7 @@
         <v>44623</v>
       </c>
       <c r="F44">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -2824,7 +2824,7 @@
         <v>44623</v>
       </c>
       <c r="F47">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -2844,7 +2844,7 @@
         <v>44623</v>
       </c>
       <c r="F48">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -2884,7 +2884,7 @@
         <v>44623</v>
       </c>
       <c r="F50">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -2904,7 +2904,7 @@
         <v>44623</v>
       </c>
       <c r="F51">
-        <v>109</v>
+        <v>116</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -2924,7 +2924,7 @@
         <v>44623</v>
       </c>
       <c r="F52">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -2944,7 +2944,7 @@
         <v>44623</v>
       </c>
       <c r="F53">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -3004,7 +3004,7 @@
         <v>44623</v>
       </c>
       <c r="F56">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -3024,7 +3024,7 @@
         <v>44623</v>
       </c>
       <c r="F57">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -3064,7 +3064,7 @@
         <v>44623</v>
       </c>
       <c r="F59">
-        <v>183</v>
+        <v>195</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -3084,7 +3084,7 @@
         <v>44623</v>
       </c>
       <c r="F60">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -3104,7 +3104,7 @@
         <v>44623</v>
       </c>
       <c r="F61">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -3124,7 +3124,7 @@
         <v>44623</v>
       </c>
       <c r="F62">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -3144,7 +3144,7 @@
         <v>44623</v>
       </c>
       <c r="F63">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -3164,7 +3164,7 @@
         <v>44623</v>
       </c>
       <c r="F64">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -3204,7 +3204,7 @@
         <v>44623</v>
       </c>
       <c r="F66">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -3244,7 +3244,7 @@
         <v>44623</v>
       </c>
       <c r="F68">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -3264,7 +3264,7 @@
         <v>44623</v>
       </c>
       <c r="F69">
-        <v>151</v>
+        <v>161</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -3344,7 +3344,7 @@
         <v>44623</v>
       </c>
       <c r="F73">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -3364,7 +3364,7 @@
         <v>44623</v>
       </c>
       <c r="F74">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -3384,7 +3384,7 @@
         <v>44623</v>
       </c>
       <c r="F75">
-        <v>124</v>
+        <v>168</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -3404,7 +3404,7 @@
         <v>44623</v>
       </c>
       <c r="F76">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -3424,7 +3424,7 @@
         <v>44623</v>
       </c>
       <c r="F77">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -3444,7 +3444,7 @@
         <v>44623</v>
       </c>
       <c r="F78">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -3464,7 +3464,7 @@
         <v>44623</v>
       </c>
       <c r="F79">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -3484,7 +3484,7 @@
         <v>44623</v>
       </c>
       <c r="F80">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -3504,7 +3504,7 @@
         <v>44623</v>
       </c>
       <c r="F81">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -3524,7 +3524,7 @@
         <v>44623</v>
       </c>
       <c r="F82">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -3544,7 +3544,7 @@
         <v>44623</v>
       </c>
       <c r="F83">
-        <v>74</v>
+        <v>85</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -3584,7 +3584,7 @@
         <v>44623</v>
       </c>
       <c r="F85">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -3604,7 +3604,7 @@
         <v>44623</v>
       </c>
       <c r="F86">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -3664,7 +3664,7 @@
         <v>44623</v>
       </c>
       <c r="F89">
-        <v>118</v>
+        <v>126</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -3704,7 +3704,7 @@
         <v>44623</v>
       </c>
       <c r="F91">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -3724,7 +3724,7 @@
         <v>44623</v>
       </c>
       <c r="F92">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="93" spans="1:6">
@@ -3764,7 +3764,7 @@
         <v>44623</v>
       </c>
       <c r="F94">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -3804,7 +3804,7 @@
         <v>44623</v>
       </c>
       <c r="F96">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="97" spans="1:6">
@@ -3884,7 +3884,7 @@
         <v>44623</v>
       </c>
       <c r="F100">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -3904,7 +3904,7 @@
         <v>44623</v>
       </c>
       <c r="F101">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -3924,7 +3924,7 @@
         <v>44623</v>
       </c>
       <c r="F102">
-        <v>40</v>
+        <v>49</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -3944,7 +3944,7 @@
         <v>44623</v>
       </c>
       <c r="F103">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -3964,7 +3964,7 @@
         <v>44623</v>
       </c>
       <c r="F104">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="105" spans="1:6">
@@ -3984,7 +3984,7 @@
         <v>44623</v>
       </c>
       <c r="F105">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -4004,7 +4004,7 @@
         <v>44623</v>
       </c>
       <c r="F106">
-        <v>145</v>
+        <v>180</v>
       </c>
     </row>
     <row r="107" spans="1:6">
@@ -4024,7 +4024,7 @@
         <v>44623</v>
       </c>
       <c r="F107">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="108" spans="1:6">
@@ -4044,7 +4044,7 @@
         <v>44623</v>
       </c>
       <c r="F108">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="109" spans="1:6">
@@ -4064,7 +4064,7 @@
         <v>44623</v>
       </c>
       <c r="F109">
-        <v>67</v>
+        <v>83</v>
       </c>
     </row>
     <row r="110" spans="1:6">
@@ -4084,7 +4084,7 @@
         <v>44623</v>
       </c>
       <c r="F110">
-        <v>112</v>
+        <v>119</v>
       </c>
     </row>
     <row r="111" spans="1:6">
@@ -4104,7 +4104,7 @@
         <v>44623</v>
       </c>
       <c r="F111">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="112" spans="1:6">
@@ -4144,7 +4144,7 @@
         <v>44623</v>
       </c>
       <c r="F113">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="114" spans="1:6">
@@ -4164,7 +4164,7 @@
         <v>44623</v>
       </c>
       <c r="F114">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="115" spans="1:6">
@@ -4264,7 +4264,7 @@
         <v>44623</v>
       </c>
       <c r="F119">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="120" spans="1:6">
@@ -4304,7 +4304,7 @@
         <v>44623</v>
       </c>
       <c r="F121">
-        <v>224</v>
+        <v>239</v>
       </c>
     </row>
     <row r="122" spans="1:6">
@@ -4324,7 +4324,7 @@
         <v>44623</v>
       </c>
       <c r="F122">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="123" spans="1:6">
@@ -4364,7 +4364,7 @@
         <v>44623</v>
       </c>
       <c r="F124">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="125" spans="1:6">
@@ -4424,7 +4424,7 @@
         <v>44623</v>
       </c>
       <c r="F127">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="128" spans="1:6">
@@ -4464,7 +4464,7 @@
         <v>44623</v>
       </c>
       <c r="F129">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="130" spans="1:6">
@@ -4504,7 +4504,7 @@
         <v>44623</v>
       </c>
       <c r="F131">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="132" spans="1:6">
@@ -4524,7 +4524,7 @@
         <v>44623</v>
       </c>
       <c r="F132">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="133" spans="1:6">
@@ -4544,7 +4544,7 @@
         <v>44623</v>
       </c>
       <c r="F133">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="134" spans="1:6">
@@ -4564,7 +4564,7 @@
         <v>44623</v>
       </c>
       <c r="F134">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="135" spans="1:6">
@@ -4584,7 +4584,7 @@
         <v>44623</v>
       </c>
       <c r="F135">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="136" spans="1:6">
@@ -4604,7 +4604,7 @@
         <v>44623</v>
       </c>
       <c r="F136">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="137" spans="1:6">
@@ -4624,7 +4624,7 @@
         <v>44623</v>
       </c>
       <c r="F137">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="138" spans="1:6">
@@ -4664,7 +4664,7 @@
         <v>44623</v>
       </c>
       <c r="F139">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="140" spans="1:6">
@@ -4684,7 +4684,7 @@
         <v>44623</v>
       </c>
       <c r="F140">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="141" spans="1:6">
@@ -4704,7 +4704,7 @@
         <v>44623</v>
       </c>
       <c r="F141">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="142" spans="1:6">
@@ -4724,7 +4724,7 @@
         <v>44623</v>
       </c>
       <c r="F142">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="143" spans="1:6">
@@ -4744,7 +4744,7 @@
         <v>44623</v>
       </c>
       <c r="F143">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="144" spans="1:6">
@@ -4764,7 +4764,7 @@
         <v>44623</v>
       </c>
       <c r="F144">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="145" spans="1:6">
@@ -4784,7 +4784,7 @@
         <v>44623</v>
       </c>
       <c r="F145">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="146" spans="1:6">
@@ -4824,7 +4824,7 @@
         <v>44623</v>
       </c>
       <c r="F147">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="148" spans="1:6">
@@ -4844,7 +4844,7 @@
         <v>44623</v>
       </c>
       <c r="F148">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="149" spans="1:6">
@@ -4864,7 +4864,7 @@
         <v>44623</v>
       </c>
       <c r="F149">
-        <v>51</v>
+        <v>58</v>
       </c>
     </row>
     <row r="150" spans="1:6">
@@ -4904,7 +4904,7 @@
         <v>44623</v>
       </c>
       <c r="F151">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="152" spans="1:6">
@@ -4924,7 +4924,7 @@
         <v>44623</v>
       </c>
       <c r="F152">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="153" spans="1:6">
@@ -4944,7 +4944,7 @@
         <v>44623</v>
       </c>
       <c r="F153">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="154" spans="1:6">
@@ -4964,7 +4964,7 @@
         <v>44623</v>
       </c>
       <c r="F154">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="155" spans="1:6">
@@ -4984,7 +4984,7 @@
         <v>44623</v>
       </c>
       <c r="F155">
-        <v>255</v>
+        <v>272</v>
       </c>
     </row>
     <row r="156" spans="1:6">
@@ -5004,7 +5004,7 @@
         <v>44623</v>
       </c>
       <c r="F156">
-        <v>83</v>
+        <v>112</v>
       </c>
     </row>
     <row r="157" spans="1:6">
@@ -5044,7 +5044,7 @@
         <v>44623</v>
       </c>
       <c r="F158">
-        <v>92</v>
+        <v>97</v>
       </c>
     </row>
     <row r="159" spans="1:6">
@@ -5084,7 +5084,7 @@
         <v>44623</v>
       </c>
       <c r="F160">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="161" spans="1:6">
@@ -5124,7 +5124,7 @@
         <v>44623</v>
       </c>
       <c r="F162">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="163" spans="1:6">
@@ -5144,7 +5144,7 @@
         <v>44623</v>
       </c>
       <c r="F163">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
     <row r="164" spans="1:6">
@@ -5184,7 +5184,7 @@
         <v>44623</v>
       </c>
       <c r="F165">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="166" spans="1:6">
@@ -5204,7 +5204,7 @@
         <v>44623</v>
       </c>
       <c r="F166">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="167" spans="1:6">
@@ -5244,7 +5244,7 @@
         <v>44623</v>
       </c>
       <c r="F168">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="169" spans="1:6">
@@ -5264,7 +5264,7 @@
         <v>44623</v>
       </c>
       <c r="F169">
-        <v>63</v>
+        <v>78</v>
       </c>
     </row>
     <row r="170" spans="1:6">
@@ -5284,7 +5284,7 @@
         <v>44623</v>
       </c>
       <c r="F170">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="171" spans="1:6">
@@ -5304,7 +5304,7 @@
         <v>44623</v>
       </c>
       <c r="F171">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="172" spans="1:6">
@@ -5344,7 +5344,7 @@
         <v>44623</v>
       </c>
       <c r="F173">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="174" spans="1:6">
@@ -5384,7 +5384,7 @@
         <v>44623</v>
       </c>
       <c r="F175">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="176" spans="1:6">
@@ -5424,7 +5424,7 @@
         <v>44623</v>
       </c>
       <c r="F177">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="178" spans="1:6">
@@ -5444,7 +5444,7 @@
         <v>44623</v>
       </c>
       <c r="F178">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="179" spans="1:6">
@@ -5484,7 +5484,7 @@
         <v>44623</v>
       </c>
       <c r="F180">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="181" spans="1:6">
@@ -5504,7 +5504,7 @@
         <v>44623</v>
       </c>
       <c r="F181">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="182" spans="1:6">
@@ -5524,7 +5524,7 @@
         <v>44623</v>
       </c>
       <c r="F182">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="183" spans="1:6">
@@ -5544,7 +5544,7 @@
         <v>44623</v>
       </c>
       <c r="F183">
-        <v>49</v>
+        <v>66</v>
       </c>
     </row>
     <row r="184" spans="1:6">
@@ -5564,7 +5564,7 @@
         <v>44623</v>
       </c>
       <c r="F184">
-        <v>96</v>
+        <v>109</v>
       </c>
     </row>
     <row r="185" spans="1:6">
@@ -5584,7 +5584,7 @@
         <v>44623</v>
       </c>
       <c r="F185">
-        <v>55</v>
+        <v>68</v>
       </c>
     </row>
     <row r="186" spans="1:6">
@@ -5624,7 +5624,7 @@
         <v>44623</v>
       </c>
       <c r="F187">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="188" spans="1:6">
@@ -5644,7 +5644,7 @@
         <v>44623</v>
       </c>
       <c r="F188">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="189" spans="1:6">
@@ -5664,7 +5664,7 @@
         <v>44623</v>
       </c>
       <c r="F189">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="190" spans="1:6">
@@ -5724,7 +5724,7 @@
         <v>44623</v>
       </c>
       <c r="F192">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="193" spans="1:6">
@@ -5744,7 +5744,7 @@
         <v>44623</v>
       </c>
       <c r="F193">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="194" spans="1:6">
@@ -5764,7 +5764,7 @@
         <v>44623</v>
       </c>
       <c r="F194">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="195" spans="1:6">
@@ -5804,7 +5804,7 @@
         <v>44623</v>
       </c>
       <c r="F196">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="197" spans="1:6">
@@ -5824,7 +5824,7 @@
         <v>44623</v>
       </c>
       <c r="F197">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="198" spans="1:6">
@@ -5844,7 +5844,7 @@
         <v>44623</v>
       </c>
       <c r="F198">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="199" spans="1:6">
@@ -5884,7 +5884,7 @@
         <v>44623</v>
       </c>
       <c r="F200">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="201" spans="1:6">
@@ -5904,7 +5904,7 @@
         <v>44623</v>
       </c>
       <c r="F201">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="202" spans="1:6">
@@ -5924,7 +5924,7 @@
         <v>44623</v>
       </c>
       <c r="F202">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="203" spans="1:6">
@@ -5944,7 +5944,7 @@
         <v>44623</v>
       </c>
       <c r="F203">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="204" spans="1:6">
@@ -5964,7 +5964,7 @@
         <v>44623</v>
       </c>
       <c r="F204">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="205" spans="1:6">
@@ -6024,7 +6024,7 @@
         <v>44623</v>
       </c>
       <c r="F207">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="208" spans="1:6">
@@ -6124,7 +6124,7 @@
         <v>44623</v>
       </c>
       <c r="F212">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="213" spans="1:6">
@@ -6144,7 +6144,7 @@
         <v>44623</v>
       </c>
       <c r="F213">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="214" spans="1:6">
@@ -6164,7 +6164,7 @@
         <v>44623</v>
       </c>
       <c r="F214">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="215" spans="1:6">
@@ -6184,7 +6184,7 @@
         <v>44623</v>
       </c>
       <c r="F215">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
     <row r="216" spans="1:6">
@@ -6204,7 +6204,7 @@
         <v>44623</v>
       </c>
       <c r="F216">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="217" spans="1:6">
@@ -6224,7 +6224,7 @@
         <v>44623</v>
       </c>
       <c r="F217">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="218" spans="1:6">
@@ -6244,7 +6244,7 @@
         <v>44623</v>
       </c>
       <c r="F218">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="219" spans="1:6">
@@ -6264,7 +6264,7 @@
         <v>44623</v>
       </c>
       <c r="F219">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="220" spans="1:6">
@@ -6284,7 +6284,7 @@
         <v>44623</v>
       </c>
       <c r="F220">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="221" spans="1:6">
@@ -6324,7 +6324,7 @@
         <v>44623</v>
       </c>
       <c r="F222">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="223" spans="1:6">
@@ -6364,7 +6364,7 @@
         <v>44623</v>
       </c>
       <c r="F224">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="225" spans="1:6">
@@ -6384,7 +6384,7 @@
         <v>44623</v>
       </c>
       <c r="F225">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="226" spans="1:6">
@@ -6404,7 +6404,7 @@
         <v>44623</v>
       </c>
       <c r="F226">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="227" spans="1:6">
@@ -6424,7 +6424,7 @@
         <v>44623</v>
       </c>
       <c r="F227">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="228" spans="1:6">
@@ -6444,7 +6444,7 @@
         <v>44623</v>
       </c>
       <c r="F228">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="229" spans="1:6">
@@ -6484,7 +6484,7 @@
         <v>44623</v>
       </c>
       <c r="F230">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="231" spans="1:6">
@@ -6544,7 +6544,7 @@
         <v>44623</v>
       </c>
       <c r="F233">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="234" spans="1:6">
@@ -6584,7 +6584,7 @@
         <v>44623</v>
       </c>
       <c r="F235">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="236" spans="1:6">
@@ -6604,7 +6604,7 @@
         <v>44623</v>
       </c>
       <c r="F236">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="237" spans="1:6">
@@ -6624,7 +6624,7 @@
         <v>44623</v>
       </c>
       <c r="F237">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>